<commit_message>
Add Download Format Data
</commit_message>
<xml_diff>
--- a/public/DataAtlet/coba.xlsx
+++ b/public/DataAtlet/coba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek Ricko\dispora-papua\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8E96C7-D66D-45A0-8B34-559091D82A31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE08F631-ABEB-4E89-BE9D-A00D434CDD50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0E50471C-7C9E-491A-A24D-1EAF7AC9CFB9}"/>
   </bookViews>
@@ -370,7 +370,7 @@
     <t>KOTA BONTANG</t>
   </si>
   <si>
-    <t>RICKY</t>
+    <t>testing</t>
   </si>
 </sst>
 </file>

</xml_diff>